<commit_message>
Adicionando dados para o curso
</commit_message>
<xml_diff>
--- a/excel_reader.xlsx
+++ b/excel_reader.xlsx
@@ -202,10 +202,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H1048576"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -321,7 +321,6 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Adicionando filtro utilizando JPQL - parte 1
</commit_message>
<xml_diff>
--- a/excel_reader.xlsx
+++ b/excel_reader.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t xml:space="preserve">2021001809</t>
   </si>
@@ -76,6 +76,15 @@
   </si>
   <si>
     <t xml:space="preserve">IFSULDEMINAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022554789</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07/05/2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matheus Franco</t>
   </si>
 </sst>
 </file>
@@ -202,10 +211,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -318,6 +327,32 @@
         <v>17</v>
       </c>
       <c r="H4" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="E5" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="F5" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>